<commit_message>
Fonts update to Open Sans
</commit_message>
<xml_diff>
--- a/roadmap.xlsx
+++ b/roadmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Мозговой штурм, получение идеи и представления  о продукте</t>
   </si>
@@ -110,12 +110,6 @@
     <t>Шрифт Consolas</t>
   </si>
   <si>
-    <t>Лицензирован по Apache license 2.0. Позволяет использование и распространение, при условии сохранения оригинальной версии, указания изменений, упоминания авторов, ознакомления пользователей с Лицензией</t>
-  </si>
-  <si>
-    <t>Лицензирован по MIT License. Позводяет свободное использование.</t>
-  </si>
-  <si>
     <t>ПО JetBrains Pycharm Professional</t>
   </si>
   <si>
@@ -138,6 +132,21 @@
   </si>
   <si>
     <t>Лицензирован собственной лицензией Microsoft. Позволяет использование в WEB, если файлы шрифтов не хранятся на сервере и не конвертируются в форматы, отличные от начальных.  https://docs.microsoft.com/en-us/typography/fonts/font-faq</t>
+  </si>
+  <si>
+    <t>Ресурс</t>
+  </si>
+  <si>
+    <t>Кол-во</t>
+  </si>
+  <si>
+    <t>Примечание</t>
+  </si>
+  <si>
+    <t>Лицензирован по Apache license 2.0, Open-Source ПО - автором является т.н. "Сообщество". Позволяет использование и распространение, при условии сохранения оригинальной версии, указания изменений, упоминания авторов, ознакомления пользователей с Лицензией</t>
+  </si>
+  <si>
+    <t>Лицензирован по MIT License, авторы Yann LeCun, Corinna Cortes, Christopher J.C. Burges. Позводяет свободное использование.</t>
   </si>
 </sst>
 </file>
@@ -234,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -401,6 +410,63 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -425,6 +491,116 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -440,7 +616,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -473,12 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,36 +659,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -808,10 +1030,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y37"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +1041,8 @@
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="67.42578125" customWidth="1"/>
-    <col min="4" max="22" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="22" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -919,7 +1142,7 @@
       <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -938,7 +1161,7 @@
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
       <c r="U3" s="14"/>
-      <c r="V3" s="31"/>
+      <c r="V3" s="33"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -948,7 +1171,7 @@
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
@@ -967,7 +1190,7 @@
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="U4" s="17"/>
-      <c r="V4" s="32"/>
+      <c r="V4" s="34"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -977,7 +1200,7 @@
       <c r="B5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="29"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="18"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -996,7 +1219,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
       <c r="U5" s="19"/>
-      <c r="V5" s="32"/>
+      <c r="V5" s="34"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -1004,7 +1227,7 @@
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="18"/>
@@ -1025,7 +1248,7 @@
       <c r="S6" s="17"/>
       <c r="T6" s="17"/>
       <c r="U6" s="17"/>
-      <c r="V6" s="32"/>
+      <c r="V6" s="34"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -1054,7 +1277,7 @@
       <c r="S7" s="17"/>
       <c r="T7" s="17"/>
       <c r="U7" s="17"/>
-      <c r="V7" s="32"/>
+      <c r="V7" s="34"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -1083,7 +1306,7 @@
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
       <c r="U8" s="17"/>
-      <c r="V8" s="32"/>
+      <c r="V8" s="34"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -1112,7 +1335,7 @@
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
       <c r="U9" s="17"/>
-      <c r="V9" s="32"/>
+      <c r="V9" s="34"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -1141,7 +1364,7 @@
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
-      <c r="V10" s="32"/>
+      <c r="V10" s="34"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -1170,7 +1393,7 @@
       <c r="S11" s="21"/>
       <c r="T11" s="17"/>
       <c r="U11" s="17"/>
-      <c r="V11" s="32"/>
+      <c r="V11" s="34"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -1199,7 +1422,7 @@
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
       <c r="U12" s="19"/>
-      <c r="V12" s="32"/>
+      <c r="V12" s="34"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -1228,7 +1451,7 @@
       <c r="S13" s="16"/>
       <c r="T13" s="16"/>
       <c r="U13" s="16"/>
-      <c r="V13" s="32"/>
+      <c r="V13" s="34"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -1257,7 +1480,7 @@
       <c r="S14" s="22"/>
       <c r="T14" s="22"/>
       <c r="U14" s="22"/>
-      <c r="V14" s="32"/>
+      <c r="V14" s="34"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -1267,7 +1490,7 @@
       <c r="B15" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="18"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -1286,7 +1509,7 @@
       <c r="S15" s="17"/>
       <c r="T15" s="17"/>
       <c r="U15" s="21"/>
-      <c r="V15" s="32"/>
+      <c r="V15" s="34"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -1374,7 +1597,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1401,468 +1624,581 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
+      <c r="B20" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="39"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="27">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
+      <c r="B21" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="32"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="44">
+        <v>3</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="26"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="45"/>
+      <c r="E23" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="26"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="27"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="45"/>
+      <c r="E24" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="26"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="60"/>
+      <c r="V25" s="61"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
+      <c r="B26" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="66"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="32"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="60"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="61"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36"/>
+      <c r="B28" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="31"/>
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
     <row r="29" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="39" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="44"/>
+      <c r="E29" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="36"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36"/>
-      <c r="U29" s="36"/>
-      <c r="V29" s="36"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="48"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="48"/>
+      <c r="T29" s="48"/>
+      <c r="U29" s="48"/>
+      <c r="V29" s="49"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="38"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="50"/>
+      <c r="E30" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="49"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="44"/>
+      <c r="E31" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="52"/>
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="27">
-        <v>2</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="26"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C33" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="34">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="44">
+        <v>2</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B34" s="20"/>
+      <c r="C34" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="54">
         <v>1</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E34" s="46" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="3:22" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="40" t="s">
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="26"/>
+    </row>
+    <row r="35" spans="1:25" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="18"/>
+      <c r="C35" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D35" s="54">
         <v>1</v>
       </c>
-      <c r="E34" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="36"/>
-      <c r="U34" s="36"/>
-      <c r="V34" s="36"/>
-    </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C35" s="41" t="s">
+      <c r="E35" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="48"/>
+      <c r="P35" s="48"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="48"/>
+      <c r="T35" s="48"/>
+      <c r="U35" s="48"/>
+      <c r="V35" s="49"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B36" s="20"/>
+      <c r="C36" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D36" s="54">
         <v>1</v>
       </c>
-      <c r="E35" s="33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C36" s="42"/>
-    </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C37" s="42" t="s">
+      <c r="E36" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="26"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="20"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="26"/>
+    </row>
+    <row r="38" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="57"/>
+      <c r="C38" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D38" s="59">
         <v>0</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" s="60" t="s">
         <v>26</v>
       </c>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E34:V34"/>
+  <mergeCells count="10">
+    <mergeCell ref="E35:V35"/>
+    <mergeCell ref="E31:V31"/>
+    <mergeCell ref="E29:V29"/>
     <mergeCell ref="E30:V30"/>
-    <mergeCell ref="E28:V28"/>
-    <mergeCell ref="E29:V29"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
License updates, no more Consolas
</commit_message>
<xml_diff>
--- a/roadmap.xlsx
+++ b/roadmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Мозговой штурм, получение идеи и представления  о продукте</t>
   </si>
@@ -95,9 +95,6 @@
     <t>MNIST Database</t>
   </si>
   <si>
-    <t>Шрифт Consolas</t>
-  </si>
-  <si>
     <t>ПО JetBrains Pycharm Professional</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
   </si>
   <si>
     <t>** информация о параметрах лицензий может быть неточна, для уточнения смотрите оригинальные файлы лицензий</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Лицензирован собственной лицензией Microsoft. Позволяет использование в WEB, если файлы шрифтов не хранятся на сервере и не конвертируются в форматы, отличные от начальных.**  https://docs.microsoft.com/en-us/typography/fonts/font-faq </t>
   </si>
   <si>
     <t>Лицензирован по MIT License, авторы Yann LeCun, Corinna Cortes, Christopher J.C. Burges. Позводяет свободное использование.**</t>
@@ -549,7 +543,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -571,19 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,21 +578,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -620,20 +590,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -671,12 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -684,6 +636,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -974,10 +962,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1071,10 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -1105,17 +1093,17 @@
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="9"/>
-      <c r="V3" s="26"/>
+      <c r="V3" s="22"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1134,17 +1122,17 @@
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
-      <c r="V4" s="27"/>
+      <c r="V4" s="23"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="13"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -1163,7 +1151,7 @@
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
-      <c r="V5" s="27"/>
+      <c r="V5" s="23"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -1171,7 +1159,7 @@
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="13"/>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="13"/>
@@ -1192,7 +1180,7 @@
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
-      <c r="V6" s="27"/>
+      <c r="V6" s="23"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -1221,7 +1209,7 @@
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
-      <c r="V7" s="27"/>
+      <c r="V7" s="23"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -1250,7 +1238,7 @@
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
-      <c r="V8" s="27"/>
+      <c r="V8" s="23"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -1279,7 +1267,7 @@
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
-      <c r="V9" s="27"/>
+      <c r="V9" s="23"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -1308,7 +1296,7 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
-      <c r="V10" s="27"/>
+      <c r="V10" s="23"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -1337,7 +1325,7 @@
       <c r="S11" s="16"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
-      <c r="V11" s="27"/>
+      <c r="V11" s="23"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -1366,7 +1354,7 @@
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="U12" s="14"/>
-      <c r="V12" s="27"/>
+      <c r="V12" s="23"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -1395,7 +1383,7 @@
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
-      <c r="V13" s="27"/>
+      <c r="V13" s="23"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -1424,36 +1412,36 @@
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
       <c r="U14" s="17"/>
-      <c r="V14" s="27"/>
+      <c r="V14" s="23"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="65"/>
-      <c r="V15" s="66"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="52"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -1514,44 +1502,44 @@
     </row>
     <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="58"/>
+      <c r="D18" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="34" t="s">
+      <c r="E18" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="33"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="27"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1569,7 +1557,7 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
-      <c r="V19" s="25"/>
+      <c r="V19" s="21"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -1580,11 +1568,11 @@
       <c r="C20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="30">
         <v>3</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
@@ -1602,7 +1590,7 @@
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
-      <c r="V20" s="21"/>
+      <c r="V20" s="19"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
@@ -1613,9 +1601,9 @@
       <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="24" t="s">
-        <v>40</v>
+      <c r="D21" s="31"/>
+      <c r="E21" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -1633,7 +1621,7 @@
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
-      <c r="V21" s="21"/>
+      <c r="V21" s="19"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
@@ -1641,12 +1629,12 @@
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="24" t="s">
-        <v>40</v>
+      <c r="D22" s="31"/>
+      <c r="E22" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1664,49 +1652,49 @@
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
       <c r="U22" s="12"/>
-      <c r="V22" s="21"/>
+      <c r="V22" s="19"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="55"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="42"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="42"/>
+      <c r="V23" s="43"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="67" t="s">
-        <v>38</v>
+      <c r="C24" s="46"/>
+      <c r="D24" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>36</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -1724,45 +1712,45 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
-      <c r="V24" s="25"/>
+      <c r="V24" s="21"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="54"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="55"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="43"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="59"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -1780,7 +1768,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="25"/>
+      <c r="V26" s="21"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
@@ -1788,30 +1776,30 @@
     <row r="27" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="43"/>
+      <c r="C27" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="55"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="55"/>
+      <c r="V27" s="56"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
@@ -1819,61 +1807,57 @@
     <row r="28" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
-      <c r="U28" s="42"/>
-      <c r="V28" s="43"/>
+      <c r="C28" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
+      <c r="V28" s="56"/>
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="15"/>
-      <c r="C29" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="46"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="19"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
@@ -1881,9 +1865,15 @@
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="47"/>
+      <c r="C30" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="30">
+        <v>2</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
@@ -1900,22 +1890,21 @@
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="U30" s="12"/>
-      <c r="V30" s="21"/>
+      <c r="V30" s="19"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
       <c r="B31" s="15"/>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="38">
-        <v>2</v>
-      </c>
-      <c r="E31" s="40" t="s">
-        <v>41</v>
+      <c r="D31" s="36">
+        <v>1</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -1933,80 +1922,71 @@
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
-      <c r="V31" s="21"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
-      <c r="C32" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="48">
+      <c r="V31" s="19"/>
+    </row>
+    <row r="32" spans="1:25" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13"/>
+      <c r="C32" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="54">
         <v>1</v>
       </c>
-      <c r="E32" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
-      <c r="S32" s="12"/>
-      <c r="T32" s="12"/>
-      <c r="U32" s="12"/>
-      <c r="V32" s="21"/>
-    </row>
-    <row r="33" spans="2:22" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
-      <c r="C33" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="68">
+      <c r="E32" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="55"/>
+      <c r="U32" s="55"/>
+      <c r="V32" s="56"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="15"/>
+      <c r="C33" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="36">
         <v>1</v>
       </c>
-      <c r="E33" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
-      <c r="S33" s="42"/>
-      <c r="T33" s="42"/>
-      <c r="U33" s="42"/>
-      <c r="V33" s="43"/>
+      <c r="E33" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="19"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
-      <c r="C34" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="48">
-        <v>1</v>
-      </c>
-      <c r="E34" s="40" t="s">
-        <v>33</v>
-      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -2023,82 +2003,58 @@
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
-      <c r="V34" s="21"/>
-    </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-      <c r="R35" s="12"/>
-      <c r="S35" s="12"/>
-      <c r="T35" s="12"/>
-      <c r="U35" s="12"/>
-      <c r="V35" s="21"/>
-    </row>
-    <row r="36" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="51"/>
-      <c r="C36" s="52" t="s">
+      <c r="V34" s="19"/>
+    </row>
+    <row r="35" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="39"/>
+      <c r="C35" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="53">
+      <c r="D35" s="41">
         <v>0</v>
       </c>
-      <c r="E36" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
-      <c r="O36" s="54"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="S36" s="54"/>
-      <c r="T36" s="54"/>
-      <c r="U36" s="54"/>
-      <c r="V36" s="55"/>
+      <c r="E35" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="42"/>
+      <c r="R35" s="42"/>
+      <c r="S35" s="42"/>
+      <c r="T35" s="42"/>
+      <c r="U35" s="42"/>
+      <c r="V35" s="43"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="29" t="s">
-        <v>31</v>
+      <c r="C38" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="E33:V33"/>
-    <mergeCell ref="E29:V29"/>
-    <mergeCell ref="E27:V27"/>
-    <mergeCell ref="E28:V28"/>
-    <mergeCell ref="B18:C18"/>
+  <mergeCells count="9">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E32:V32"/>
+    <mergeCell ref="E27:V27"/>
+    <mergeCell ref="E28:V28"/>
+    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
One more roadmap update
</commit_message>
<xml_diff>
--- a/roadmap.xlsx
+++ b/roadmap.xlsx
@@ -702,79 +702,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -785,21 +746,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -822,19 +774,67 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1129,15 +1129,15 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="23" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1237,11 +1237,11 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1267,11 +1267,11 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -1297,11 +1297,11 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
       <c r="E5" s="13"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -1328,10 +1328,10 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="13"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="13"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -1358,10 +1358,10 @@
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="15"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1388,10 +1388,10 @@
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="15"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1418,10 +1418,10 @@
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="15"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1448,10 +1448,10 @@
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="15"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1478,10 +1478,10 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="15"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1508,10 +1508,10 @@
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="15"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1538,10 +1538,10 @@
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="35"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="15"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -1568,10 +1568,10 @@
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="35"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="15"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -1590,25 +1590,25 @@
       <c r="T14" s="16"/>
       <c r="U14" s="16"/>
       <c r="V14" s="16"/>
-      <c r="W14" s="70"/>
+      <c r="W14" s="54"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
       <c r="E15" s="28"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
@@ -1619,8 +1619,8 @@
       <c r="S15" s="26"/>
       <c r="T15" s="26"/>
       <c r="U15" s="26"/>
-      <c r="V15" s="68"/>
-      <c r="W15" s="69"/>
+      <c r="V15" s="52"/>
+      <c r="W15" s="53"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
@@ -1683,46 +1683,46 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="45" t="s">
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
-      <c r="T18" s="46"/>
-      <c r="U18" s="46"/>
-      <c r="V18" s="46"/>
-      <c r="W18" s="47"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="34"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="48"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
@@ -1740,19 +1740,19 @@
       <c r="T19" s="27"/>
       <c r="U19" s="27"/>
       <c r="V19" s="27"/>
-      <c r="W19" s="49"/>
+      <c r="W19" s="36"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="37" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="51">
+      <c r="D20" s="61"/>
+      <c r="E20" s="38">
         <v>3</v>
       </c>
       <c r="F20" s="23" t="s">
@@ -1774,19 +1774,19 @@
       <c r="T20" s="23"/>
       <c r="U20" s="23"/>
       <c r="V20" s="23"/>
-      <c r="W20" s="52"/>
+      <c r="W20" s="39"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="37" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="51"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="23" t="s">
         <v>45</v>
       </c>
@@ -1806,19 +1806,19 @@
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
       <c r="V21" s="23"/>
-      <c r="W21" s="52"/>
+      <c r="W21" s="39"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="39" t="s">
+      <c r="B22" s="37"/>
+      <c r="C22" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="51"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="38"/>
       <c r="F22" s="23" t="s">
         <v>45</v>
       </c>
@@ -1837,17 +1837,17 @@
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
       <c r="V22" s="23"/>
-      <c r="W22" s="52"/>
+      <c r="W22" s="39"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="53"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
-      <c r="E23" s="54"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="25"/>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
@@ -1865,22 +1865,22 @@
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="55"/>
+      <c r="W23" s="42"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="55" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="43" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="27"/>
@@ -1899,17 +1899,17 @@
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
-      <c r="W24" s="49"/>
+      <c r="W24" s="36"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="53"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="54"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -1927,19 +1927,19 @@
       <c r="T25" s="25"/>
       <c r="U25" s="25"/>
       <c r="V25" s="25"/>
-      <c r="W25" s="55"/>
+      <c r="W25" s="42"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="55" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="48"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
@@ -1957,82 +1957,82 @@
       <c r="T26" s="27"/>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
-      <c r="W26" s="49"/>
+      <c r="W26" s="36"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="37" t="s">
+      <c r="B27" s="37"/>
+      <c r="C27" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="57" t="s">
+      <c r="D27" s="61"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="57"/>
-      <c r="P27" s="57"/>
-      <c r="Q27" s="57"/>
-      <c r="R27" s="57"/>
-      <c r="S27" s="57"/>
-      <c r="T27" s="57"/>
-      <c r="U27" s="57"/>
-      <c r="V27" s="57"/>
-      <c r="W27" s="58"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="63"/>
+      <c r="V27" s="63"/>
+      <c r="W27" s="64"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="37" t="s">
+      <c r="B28" s="37"/>
+      <c r="C28" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="57" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
-      <c r="V28" s="57"/>
-      <c r="W28" s="58"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="63"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="64"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="50"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="23"/>
       <c r="D29" s="23"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="60"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
@@ -2049,19 +2049,19 @@
       <c r="T29" s="23"/>
       <c r="U29" s="23"/>
       <c r="V29" s="23"/>
-      <c r="W29" s="52"/>
+      <c r="W29" s="39"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="37" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="51">
+      <c r="D30" s="61"/>
+      <c r="E30" s="38">
         <v>2</v>
       </c>
       <c r="F30" s="24" t="s">
@@ -2083,18 +2083,18 @@
       <c r="T30" s="23"/>
       <c r="U30" s="23"/>
       <c r="V30" s="23"/>
-      <c r="W30" s="52"/>
+      <c r="W30" s="39"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B31" s="50"/>
-      <c r="C31" s="37" t="s">
+      <c r="B31" s="37"/>
+      <c r="C31" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="41">
+      <c r="D31" s="61"/>
+      <c r="E31" s="30">
         <v>1</v>
       </c>
       <c r="F31" s="24" t="s">
@@ -2116,69 +2116,69 @@
       <c r="T31" s="23"/>
       <c r="U31" s="23"/>
       <c r="V31" s="23"/>
-      <c r="W31" s="52"/>
+      <c r="W31" s="39"/>
     </row>
     <row r="32" spans="1:26" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="50"/>
-      <c r="C32" s="39" t="s">
+      <c r="B32" s="37"/>
+      <c r="C32" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="57" t="s">
+      <c r="D32" s="57"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
-      <c r="S32" s="57"/>
-      <c r="T32" s="57"/>
-      <c r="U32" s="57"/>
-      <c r="V32" s="57"/>
-      <c r="W32" s="58"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="63"/>
+      <c r="V32" s="63"/>
+      <c r="W32" s="64"/>
     </row>
     <row r="33" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="50"/>
-      <c r="C33" s="39" t="s">
+      <c r="B33" s="37"/>
+      <c r="C33" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="61" t="s">
+      <c r="D33" s="57"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="57"/>
-      <c r="P33" s="57"/>
-      <c r="Q33" s="57"/>
-      <c r="R33" s="57"/>
-      <c r="S33" s="57"/>
-      <c r="T33" s="57"/>
-      <c r="U33" s="57"/>
-      <c r="V33" s="57"/>
-      <c r="W33" s="58"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="63"/>
+      <c r="V33" s="63"/>
+      <c r="W33" s="64"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="50"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="23"/>
       <c r="D34" s="23"/>
-      <c r="E34" s="51"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
@@ -2196,210 +2196,210 @@
       <c r="T34" s="23"/>
       <c r="U34" s="23"/>
       <c r="V34" s="23"/>
-      <c r="W34" s="52"/>
+      <c r="W34" s="39"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="62"/>
-      <c r="C35" s="37" t="s">
+      <c r="B35" s="46"/>
+      <c r="C35" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="36"/>
-      <c r="P35" s="36"/>
-      <c r="Q35" s="36"/>
-      <c r="R35" s="36"/>
-      <c r="S35" s="36"/>
-      <c r="T35" s="36"/>
-      <c r="U35" s="36"/>
-      <c r="V35" s="36"/>
-      <c r="W35" s="65"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
+      <c r="T35" s="29"/>
+      <c r="U35" s="29"/>
+      <c r="V35" s="29"/>
+      <c r="W35" s="49"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="62"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42" t="s">
+      <c r="B36" s="46"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="64" t="s">
+      <c r="E36" s="47"/>
+      <c r="F36" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="36"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="T36" s="36"/>
-      <c r="U36" s="36"/>
-      <c r="V36" s="36"/>
-      <c r="W36" s="65"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="49"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="62"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36" t="s">
+      <c r="B37" s="46"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="64" t="s">
+      <c r="E37" s="47"/>
+      <c r="F37" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="36"/>
-      <c r="V37" s="36"/>
-      <c r="W37" s="65"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="49"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="62"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36" t="s">
+      <c r="B38" s="46"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="64" t="s">
+      <c r="E38" s="47"/>
+      <c r="F38" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="36"/>
-      <c r="T38" s="36"/>
-      <c r="U38" s="36"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="65"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="49"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="62"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36" t="s">
+      <c r="B39" s="46"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="64" t="s">
+      <c r="E39" s="47"/>
+      <c r="F39" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="65"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="49"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="62"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36" t="s">
+      <c r="B40" s="46"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="63"/>
-      <c r="F40" s="64" t="s">
+      <c r="E40" s="47"/>
+      <c r="F40" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="T40" s="36"/>
-      <c r="U40" s="36"/>
-      <c r="V40" s="36"/>
-      <c r="W40" s="65"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="49"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="62"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36" t="s">
+      <c r="B41" s="46"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="63">
+      <c r="E41" s="47">
         <v>3</v>
       </c>
-      <c r="F41" s="64" t="s">
+      <c r="F41" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="S41" s="36"/>
-      <c r="T41" s="36"/>
-      <c r="U41" s="36"/>
-      <c r="V41" s="36"/>
-      <c r="W41" s="65"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="29"/>
+      <c r="T41" s="29"/>
+      <c r="U41" s="29"/>
+      <c r="V41" s="29"/>
+      <c r="W41" s="49"/>
     </row>
     <row r="42" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="53"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="67"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="51"/>
       <c r="G42" s="25"/>
       <c r="H42" s="25"/>
       <c r="I42" s="25"/>
@@ -2416,7 +2416,7 @@
       <c r="T42" s="25"/>
       <c r="U42" s="25"/>
       <c r="V42" s="25"/>
-      <c r="W42" s="55"/>
+      <c r="W42" s="42"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
@@ -2435,11 +2435,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F33:W33"/>
-    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B15:D15"/>
@@ -2453,10 +2448,15 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F33:W33"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="F32:W32"/>
     <mergeCell ref="F27:W27"/>
     <mergeCell ref="F28:W28"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>

</xml_diff>